<commit_message>
Add RunExamples, add proper comments,  fixed runtime errors and fixed namespace issue
</commit_message>
<xml_diff>
--- a/Examples/Data/Articles/CombineMultipleWorksheetsSingleWorksheet/Output.xlsx
+++ b/Examples/Data/Articles/CombineMultipleWorksheetsSingleWorksheet/Output.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Evaluation Warning" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Evaluation Warning" sheetId="2" r:id="rId3"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId6"/>
@@ -21,25 +21,27 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>Evaluation Only. Created with Aspose.Cells for .NET.Copyright 2003 - 2014 Aspose Pty Ltd.</t>
+    <t>Evaluation Only. Created with Aspose.Cells for .NET.Copyright 2003 - 2016 Aspose Pty Ltd.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <b/>
+      <i/>
+      <sz val="18"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -50,10 +52,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <i/>
-      <sz val="18"/>
-      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -99,21 +105,21 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
       <alignment/>
       <protection/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="20" applyFont="1">
       <alignment/>
       <protection/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment/>
       <protection/>
     </xf>
@@ -203,7 +209,7 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c:style val="102"/>
+      <c14:style val="102"/>
     </mc:Choice>
     <mc:Fallback>
       <c:style val="2"/>
@@ -230,12 +236,13 @@
         <a:solidFill>
           <a:srgbClr val="C0C0C0"/>
         </a:solidFill>
-        <a:ln w="3175">
+        <a:ln w="3175" cap="flat" cmpd="sng">
           <a:solidFill>
             <a:srgbClr val="000000"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
+        <a:effectLst/>
       </c:spPr>
     </c:backWall>
     <c:plotArea>
@@ -261,22 +268,40 @@
             <a:solidFill>
               <a:srgbClr val="9999FF"/>
             </a:solidFill>
-            <a:ln w="12700">
+            <a:ln w="12700" cap="flat" cmpd="sng">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
               <a:prstDash val="solid"/>
             </a:ln>
+            <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:numFmt formatCode="General" sourceLinked="1"/>
-            <c:delete val="1"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$A$1:$A$3</c:f>
-              <c:numCache/>
+              <c:numCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
           <c:shape val="pyramid"/>
@@ -288,98 +313,151 @@
             <a:solidFill>
               <a:srgbClr val="993366"/>
             </a:solidFill>
-            <a:ln w="12700">
+            <a:ln w="12700" cap="flat" cmpd="sng">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
               <a:prstDash val="solid"/>
             </a:ln>
+            <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:numFmt formatCode="General" sourceLinked="1"/>
-            <c:delete val="1"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$B$1:$B$3</c:f>
-              <c:numCache/>
+              <c:numCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
           <c:shape val="pyramid"/>
         </c:ser>
         <c:shape val="pyramid"/>
-        <c:axId val="17940955"/>
-        <c:axId val="59835590"/>
+        <c:axId val="30542218"/>
+        <c:axId val="6444509"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="17940955"/>
+        <c:axId val="30542218"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:delete val="0"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln w="3175">
+          <a:ln w="3175" cap="flat" cmpd="sng">
             <a:solidFill>
               <a:srgbClr val="000000"/>
             </a:solidFill>
             <a:prstDash val="solid"/>
           </a:ln>
+          <a:effectLst/>
         </c:spPr>
-        <c:crossAx val="59835590"/>
+        <c:txPr>
+          <a:bodyPr vert="horz" rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="Arial"/>
+                <a:cs typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="6444509"/>
         <c:crosses val="autoZero"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="59835590"/>
+        <c:axId val="6444509"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln w="3175">
+            <a:ln w="3175" cap="flat" cmpd="sng">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
               <a:prstDash val="solid"/>
             </a:ln>
+            <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:delete val="0"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln w="3175">
+          <a:ln w="3175" cap="flat" cmpd="sng">
             <a:solidFill>
               <a:srgbClr val="000000"/>
             </a:solidFill>
             <a:prstDash val="solid"/>
           </a:ln>
+          <a:effectLst/>
         </c:spPr>
-        <c:crossAx val="17940955"/>
+        <c:txPr>
+          <a:bodyPr vert="horz" rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="Arial"/>
+                <a:cs typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="30542218"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:dispUnits/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
           <a:srgbClr val="C0C0C0"/>
         </a:solidFill>
-        <a:ln w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng">
           <a:solidFill>
             <a:srgbClr val="808080"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
+        <a:effectLst/>
       </c:spPr>
     </c:plotArea>
     <c:legend>
@@ -399,12 +477,13 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="3175">
+        <a:ln w="3175" cap="flat" cmpd="sng">
           <a:solidFill>
             <a:srgbClr val="000000"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
+        <a:effectLst/>
       </c:spPr>
       <c:txPr>
         <a:bodyPr vert="horz" rot="0"/>
@@ -425,17 +504,19 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
       <a:srgbClr val="FFFFFF"/>
     </a:solidFill>
-    <a:ln w="3175">
+    <a:ln w="3175" cap="flat" cmpd="sng">
       <a:solidFill>
         <a:srgbClr val="000000"/>
       </a:solidFill>
       <a:prstDash val="solid"/>
     </a:ln>
+    <a:effectLst/>
   </c:spPr>
   <c:txPr>
     <a:bodyPr vert="horz" rot="0"/>
@@ -461,7 +542,7 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c:style val="102"/>
+      <c14:style val="102"/>
     </mc:Choice>
     <mc:Fallback>
       <c:style val="2"/>
@@ -488,20 +569,26 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="12700">
+            <a:ln w="12700" cmpd="sng">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
               <a:prstDash val="solid"/>
             </a:ln>
+            <a:effectLst/>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
             <c:numFmt formatCode="General" sourceLinked="1"/>
-            <c:showLeaderLines val="1"/>
-            <c:delete val="1"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -549,20 +636,26 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:spPr>
-            <a:ln w="12700">
+            <a:ln w="12700" cmpd="sng">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
               <a:prstDash val="solid"/>
             </a:ln>
+            <a:effectLst/>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
             <c:numFmt formatCode="General" sourceLinked="1"/>
-            <c:showLeaderLines val="1"/>
-            <c:delete val="1"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -607,77 +700,112 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="66433212"/>
-        <c:axId val="42109742"/>
+        <c:axId val="58000584"/>
+        <c:axId val="52243212"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="66433212"/>
+        <c:axId val="58000584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:delete val="0"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln w="3175">
+          <a:ln w="3175" cap="flat" cmpd="sng">
             <a:solidFill>
               <a:srgbClr val="000000"/>
             </a:solidFill>
             <a:prstDash val="solid"/>
           </a:ln>
+          <a:effectLst/>
         </c:spPr>
-        <c:crossAx val="42109742"/>
+        <c:txPr>
+          <a:bodyPr vert="horz" rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="Arial"/>
+                <a:cs typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="52243212"/>
         <c:crosses val="autoZero"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="42109742"/>
+        <c:axId val="52243212"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln w="3175">
+            <a:ln w="3175" cap="flat" cmpd="sng">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
               <a:prstDash val="solid"/>
             </a:ln>
+            <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:delete val="0"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln w="3175">
+          <a:ln w="3175" cap="flat" cmpd="sng">
             <a:solidFill>
               <a:srgbClr val="000000"/>
             </a:solidFill>
             <a:prstDash val="solid"/>
           </a:ln>
+          <a:effectLst/>
         </c:spPr>
-        <c:crossAx val="66433212"/>
+        <c:txPr>
+          <a:bodyPr vert="horz" rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="Arial"/>
+                <a:cs typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="58000584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:dispUnits/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
           <a:srgbClr val="C0C0C0"/>
         </a:solidFill>
-        <a:ln w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng">
           <a:solidFill>
             <a:srgbClr val="808080"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
+        <a:effectLst/>
       </c:spPr>
     </c:plotArea>
     <c:legend>
@@ -697,12 +825,13 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="3175">
+        <a:ln w="3175" cap="flat" cmpd="sng">
           <a:solidFill>
             <a:srgbClr val="000000"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
+        <a:effectLst/>
       </c:spPr>
       <c:txPr>
         <a:bodyPr vert="horz" rot="0"/>
@@ -723,17 +852,19 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
       <a:srgbClr val="FFFFFF"/>
     </a:solidFill>
-    <a:ln w="3175">
+    <a:ln w="3175" cap="flat" cmpd="sng">
       <a:solidFill>
         <a:srgbClr val="000000"/>
       </a:solidFill>
       <a:prstDash val="solid"/>
     </a:ln>
+    <a:effectLst/>
   </c:spPr>
   <c:txPr>
     <a:bodyPr vert="horz" rot="0"/>
@@ -755,7 +886,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -848,7 +979,6 @@
           <a:ext cx="2466975" cy="1847850"/>
         </a:xfrm>
         <a:prstGeom prst="rect"/>
-        <a:noFill/>
         <a:ln w="9525" cmpd="sng">
           <a:noFill/>
         </a:ln>
@@ -867,6 +997,56 @@
       <sheetName val="Sheet2"/>
       <sheetName val="Evaluation Warning"/>
     </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="1">
+          <cell r="A1">
+            <v>50</v>
+          </cell>
+          <cell r="B1">
+            <v>60</v>
+          </cell>
+          <cell r="C1" t="str">
+            <v>Q1</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2">
+            <v>100</v>
+          </cell>
+          <cell r="B2">
+            <v>32</v>
+          </cell>
+          <cell r="C2" t="str">
+            <v>Q2</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3">
+            <v>150</v>
+          </cell>
+          <cell r="B3">
+            <v>50</v>
+          </cell>
+          <cell r="C3" t="str">
+            <v>Y1</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4">
+            <v>200</v>
+          </cell>
+          <cell r="B4">
+            <v>40</v>
+          </cell>
+          <cell r="C4" t="str">
+            <v>Y2</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2"/>
+    </sheetDataSet>
   </externalBook>
 </externalLink>
 </file>
@@ -1190,15 +1370,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
-  <cols>
-    <col min="1" max="11" width="9.14285714285714" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData>
     <row r="1" spans="1:2" ht="12.75">
       <c r="A1" s="1">
@@ -1229,18 +1406,18 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageSetup orientation="portrait"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A5:A5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <dimension ref="A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData>
     <row r="5" ht="23.25" customHeight="1">
       <c r="A5" s="3" t="s">
@@ -1249,6 +1426,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>